<commit_message>
Added , on_duplicate_key_ignore: true,  track_validation_failures: true for imports
</commit_message>
<xml_diff>
--- a/public/sample_uploads/account_entries.xlsx
+++ b/public/sample_uploads/account_entries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04C8F2BA-1A81-464C-B645-271A1A2496D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B53163-3B84-4A54-BEB9-A179CA1A82A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{1421E284-CBF3-4912-9765-3F7D17EF0783}"/>
   </bookViews>
@@ -484,7 +484,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -524,26 +524,26 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="3">
-        <v>6</v>
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
       </c>
       <c r="D2" s="1">
-        <v>44960</v>
+        <v>44961</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="G2">
-        <v>1000</v>
+        <v>0.06</v>
       </c>
       <c r="I2" t="s">
         <v>19</v>
@@ -551,28 +551,25 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="1">
         <v>44960</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G3">
-        <v>2000</v>
-      </c>
-      <c r="H3" t="s">
-        <v>12</v>
+        <v>1000</v>
       </c>
       <c r="I3" t="s">
         <v>19</v>
@@ -592,13 +589,16 @@
         <v>44960</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G4">
-        <v>1000</v>
+        <v>2000</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
       </c>
       <c r="I4" t="s">
         <v>19</v>
@@ -606,16 +606,16 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="1">
-        <v>44961</v>
+        <v>44960</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
@@ -632,28 +632,25 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="1">
         <v>44961</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G6">
-        <v>2000</v>
-      </c>
-      <c r="H6" t="s">
-        <v>12</v>
+        <v>1000</v>
       </c>
       <c r="I6" t="s">
         <v>19</v>
@@ -673,13 +670,16 @@
         <v>44961</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G7">
-        <v>1000</v>
+        <v>2000</v>
+      </c>
+      <c r="H7" t="s">
+        <v>12</v>
       </c>
       <c r="I7" t="s">
         <v>19</v>
@@ -693,7 +693,7 @@
         <v>14</v>
       </c>
       <c r="C8" s="3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" s="1">
         <v>44961</v>
@@ -713,25 +713,25 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="3">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D9" s="1">
-        <v>44960</v>
+        <v>44961</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="G9">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="I9" t="s">
         <v>19</v>
@@ -739,13 +739,13 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D10" s="1">
         <v>44960</v>
@@ -765,16 +765,16 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11" s="1">
-        <v>44961</v>
+        <v>44960</v>
       </c>
       <c r="E11" t="s">
         <v>20</v>
@@ -791,13 +791,13 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D12" s="1">
         <v>44961</v>
@@ -823,7 +823,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D13" s="1">
         <v>44961</v>
@@ -843,25 +843,25 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="3">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D14" s="1">
-        <v>44960</v>
+        <v>44961</v>
       </c>
       <c r="E14" t="s">
         <v>20</v>
       </c>
       <c r="F14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G14">
-        <v>0.05</v>
+        <v>500</v>
       </c>
       <c r="I14" t="s">
         <v>19</v>
@@ -869,13 +869,13 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D15" s="1">
         <v>44960</v>
@@ -887,7 +887,7 @@
         <v>22</v>
       </c>
       <c r="G15">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="I15" t="s">
         <v>19</v>
@@ -895,16 +895,16 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D16" s="1">
-        <v>44961</v>
+        <v>44960</v>
       </c>
       <c r="E16" t="s">
         <v>20</v>
@@ -913,7 +913,7 @@
         <v>22</v>
       </c>
       <c r="G16">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="I16" t="s">
         <v>19</v>
@@ -921,13 +921,13 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D17" s="1">
         <v>44961</v>
@@ -939,21 +939,21 @@
         <v>22</v>
       </c>
       <c r="G17">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="I17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
+      <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18">
-        <v>10</v>
+      <c r="B18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="3">
+        <v>9</v>
       </c>
       <c r="D18" s="1">
         <v>44961</v>

</xml_diff>

<commit_message>
import hssets with comments in headers
</commit_message>
<xml_diff>
--- a/public/sample_uploads/account_entries.xlsx
+++ b/public/sample_uploads/account_entries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aseem Karmali\Desktop\bulk files with notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56328380-6BAA-4E61-9F47-03491A0D3350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C79764-77F6-4161-966E-39A96349BBF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{1421E284-CBF3-4912-9765-3F7D17EF0783}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{1421E284-CBF3-4912-9765-3F7D17EF0783}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,238 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{CF638530-D0C9-4268-A05D-4ADA1F61539A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+-Investor name as recorded on CapHive is mandatory incase account entry pertains to a specific investor
+-Leave blank incase account entry pertains to a fund / scheme</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{F34029CD-F05D-462C-ABEB-FA94CB764D77}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Mandatory: Fund name recorded on CapHive</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{CB5C4B9E-E495-40F0-A1C7-3294BBCE90E1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Mandatory, needed for mapping to the appropriate folio.  
+If needed you may download the list of commiments which will give the Investor Name and Folio No.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{BC632EDF-CF97-436F-BDA0-5945484A07D9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Mandatory in dd/mm/yyyy format</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{C2C3E7E0-5201-4EFF-A78A-36F29C0272E0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+-Mandatory 
+-Please use the existing nomenclature as shown by CapHive</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{C0252432-4D8E-47C7-831B-22D508FAC953}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+-Mandatory 
+-Please use the existing nomenclature as shown by CapHive</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{F9983D45-2BF0-4844-9767-A07FC9C0B44F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+-Mandatory
+-Incase of a percentage - please put the exact value i.e. 0.06 for 6%</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{914B8BE3-84D1-4DA5-9E4C-1617DB28A883}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+-Optional</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{9D9603A5-6ED9-4461-9057-2C7332180EE0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+-Mandatory
+-Please use the existing nomenclature as shown by CapHive</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="25">
   <si>
@@ -115,7 +347,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,6 +371,38 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -148,12 +412,21 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -164,11 +437,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,72 +761,79 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFD405DB-DFFA-46CC-B3D6-72FB3274A2C6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFD405DB-DFFA-46CC-B3D6-72FB3274A2C6}">
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.9296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.46484375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.53125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.06640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2">
         <v>10</v>
       </c>
-      <c r="D2" s="1">
-        <v>44961</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" s="5">
+        <v>45018</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="2">
         <v>0.06</v>
       </c>
-      <c r="I2" t="s">
+      <c r="H2" s="2"/>
+      <c r="I2" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -559,25 +841,26 @@
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="3">
         <v>6</v>
       </c>
-      <c r="D3" s="1">
-        <v>44960</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" s="5">
+        <v>44987</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2">
         <v>1000</v>
       </c>
-      <c r="I3" t="s">
+      <c r="H3" s="2"/>
+      <c r="I3" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -585,28 +868,28 @@
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="3">
         <v>7</v>
       </c>
-      <c r="D4" s="1">
-        <v>44960</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D4" s="5">
+        <v>44987</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <v>2000</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -614,25 +897,26 @@
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="3">
         <v>7</v>
       </c>
-      <c r="D5" s="1">
-        <v>44960</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="D5" s="5">
+        <v>44987</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="2">
         <v>1000</v>
       </c>
-      <c r="I5" t="s">
+      <c r="H5" s="2"/>
+      <c r="I5" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -640,25 +924,26 @@
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="3">
         <v>8</v>
       </c>
-      <c r="D6" s="1">
-        <v>44961</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D6" s="5">
+        <v>45018</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="2">
         <v>1000</v>
       </c>
-      <c r="I6" t="s">
+      <c r="H6" s="2"/>
+      <c r="I6" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -666,28 +951,28 @@
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="3">
         <v>9</v>
       </c>
-      <c r="D7" s="1">
-        <v>44961</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D7" s="5">
+        <v>45018</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <v>2000</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -695,25 +980,26 @@
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="3">
         <v>9</v>
       </c>
-      <c r="D8" s="1">
-        <v>44961</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="D8" s="5">
+        <v>45018</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="2">
         <v>1000</v>
       </c>
-      <c r="I8" t="s">
+      <c r="H8" s="2"/>
+      <c r="I8" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -721,25 +1007,26 @@
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="3">
         <v>10</v>
       </c>
-      <c r="D9" s="1">
-        <v>44961</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="D9" s="5">
+        <v>45018</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="2">
         <v>1000</v>
       </c>
-      <c r="I9" t="s">
+      <c r="H9" s="2"/>
+      <c r="I9" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -747,25 +1034,26 @@
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="3">
         <v>6</v>
       </c>
-      <c r="D10" s="1">
-        <v>44960</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="D10" s="5">
+        <v>44987</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="2">
         <v>500</v>
       </c>
-      <c r="I10" t="s">
+      <c r="H10" s="2"/>
+      <c r="I10" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -773,25 +1061,26 @@
       <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="3">
         <v>7</v>
       </c>
-      <c r="D11" s="1">
-        <v>44960</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="D11" s="5">
+        <v>44987</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="2">
         <v>500</v>
       </c>
-      <c r="I11" t="s">
+      <c r="H11" s="2"/>
+      <c r="I11" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -799,25 +1088,26 @@
       <c r="A12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="3">
         <v>8</v>
       </c>
-      <c r="D12" s="1">
-        <v>44961</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="D12" s="5">
+        <v>45018</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="2">
         <v>500</v>
       </c>
-      <c r="I12" t="s">
+      <c r="H12" s="2"/>
+      <c r="I12" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -825,25 +1115,26 @@
       <c r="A13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="3">
         <v>9</v>
       </c>
-      <c r="D13" s="1">
-        <v>44961</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="D13" s="5">
+        <v>45018</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="2">
         <v>500</v>
       </c>
-      <c r="I13" t="s">
+      <c r="H13" s="2"/>
+      <c r="I13" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -851,25 +1142,26 @@
       <c r="A14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="3">
         <v>10</v>
       </c>
-      <c r="D14" s="1">
-        <v>44961</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="D14" s="5">
+        <v>45018</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="2">
         <v>500</v>
       </c>
-      <c r="I14" t="s">
+      <c r="H14" s="2"/>
+      <c r="I14" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -877,25 +1169,26 @@
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="3">
         <v>6</v>
       </c>
-      <c r="D15" s="1">
-        <v>44960</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="D15" s="5">
+        <v>44987</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="2">
         <v>0.05</v>
       </c>
-      <c r="I15" t="s">
+      <c r="H15" s="2"/>
+      <c r="I15" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -903,25 +1196,26 @@
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="3">
         <v>7</v>
       </c>
-      <c r="D16" s="1">
-        <v>44960</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="D16" s="5">
+        <v>44987</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="2">
         <v>0.06</v>
       </c>
-      <c r="I16" t="s">
+      <c r="H16" s="2"/>
+      <c r="I16" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -929,25 +1223,26 @@
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="3">
         <v>8</v>
       </c>
-      <c r="D17" s="1">
-        <v>44961</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="D17" s="5">
+        <v>45018</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="2">
         <v>0.05</v>
       </c>
-      <c r="I17" t="s">
+      <c r="H17" s="2"/>
+      <c r="I17" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -955,25 +1250,26 @@
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="3">
         <v>9</v>
       </c>
-      <c r="D18" s="1">
-        <v>44961</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="D18" s="5">
+        <v>45018</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="2">
         <v>0.06</v>
       </c>
-      <c r="I18" t="s">
+      <c r="H18" s="2"/>
+      <c r="I18" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -981,25 +1277,26 @@
       <c r="A19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="3">
         <v>11</v>
       </c>
-      <c r="D19" s="1">
-        <v>44961</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="D19" s="5">
+        <v>45018</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="2">
         <v>0.06</v>
       </c>
-      <c r="I19" t="s">
+      <c r="H19" s="2"/>
+      <c r="I19" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1007,29 +1304,36 @@
       <c r="A20" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C20" s="3">
         <v>12</v>
       </c>
-      <c r="D20" s="1">
-        <v>44961</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="D20" s="5">
+        <v>45018</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="2">
         <v>0.06</v>
       </c>
-      <c r="I20" t="s">
+      <c r="H20" s="2"/>
+      <c r="I20" s="2" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576" xr:uid="{E4F543E0-B5B2-429B-9B62-7D17366B8716}">
+      <formula1>"Pool,All"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Portfolio llm report (#534)
* Added rule for in import

* raise errors if fund or CD is not found

* display custom fields in CDP

* Added Rule for

* Added includes to load associations

* Added job to generate portfolio report from folder

* Added Generate Report btn to folder in investor

* Added pulling of docx format of the report
</commit_message>
<xml_diff>
--- a/public/sample_uploads/account_entries.xlsx
+++ b/public/sample_uploads/account_entries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aseem Karmali\Desktop\bulk files with notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C79764-77F6-4161-966E-39A96349BBF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D9EA23-26F5-4356-8F5B-142DFC528269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{1421E284-CBF3-4912-9765-3F7D17EF0783}"/>
+    <workbookView xWindow="15" yWindow="735" windowWidth="23985" windowHeight="14265" xr2:uid="{1421E284-CBF3-4912-9765-3F7D17EF0783}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -266,7 +266,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="28">
   <si>
     <t>Investor *</t>
   </si>
@@ -341,6 +341,15 @@
   </si>
   <si>
     <t>Investor 6</t>
+  </si>
+  <si>
+    <t>Rule For</t>
+  </si>
+  <si>
+    <t>Accounting</t>
+  </si>
+  <si>
+    <t>Reporting</t>
   </si>
 </sst>
 </file>
@@ -437,13 +446,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -762,10 +772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFD405DB-DFFA-46CC-B3D6-72FB3274A2C6}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="J4" sqref="J4:J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -781,7 +791,7 @@
     <col min="9" max="9" width="5.06640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -809,8 +819,11 @@
       <c r="I1" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J1" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -836,8 +849,11 @@
       <c r="I2" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J2" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -863,8 +879,11 @@
       <c r="I3" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J3" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
@@ -892,8 +911,11 @@
       <c r="I4" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J4" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -919,8 +941,11 @@
       <c r="I5" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J5" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -946,8 +971,11 @@
       <c r="I6" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J6" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
@@ -975,8 +1003,11 @@
       <c r="I7" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J7" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
@@ -1002,8 +1033,11 @@
       <c r="I8" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J8" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -1029,8 +1063,11 @@
       <c r="I9" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J9" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
@@ -1056,8 +1093,11 @@
       <c r="I10" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J10" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
@@ -1083,8 +1123,11 @@
       <c r="I11" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J11" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>16</v>
       </c>
@@ -1110,8 +1153,11 @@
       <c r="I12" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J12" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>17</v>
       </c>
@@ -1137,8 +1183,11 @@
       <c r="I13" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J13" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>17</v>
       </c>
@@ -1164,8 +1213,11 @@
       <c r="I14" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J14" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
@@ -1191,8 +1243,11 @@
       <c r="I15" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J15" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -1218,8 +1273,11 @@
       <c r="I16" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J16" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
@@ -1245,8 +1303,11 @@
       <c r="I17" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J17" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -1272,8 +1333,11 @@
       <c r="I18" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J18" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>23</v>
       </c>
@@ -1299,8 +1363,11 @@
       <c r="I19" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J19" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>24</v>
       </c>
@@ -1325,6 +1392,9 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2" t="s">
         <v>19</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed Account entries rule_for for import, updated excel (#538)
</commit_message>
<xml_diff>
--- a/public/sample_uploads/account_entries.xlsx
+++ b/public/sample_uploads/account_entries.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aseem Karmali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D9EA23-26F5-4356-8F5B-142DFC528269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A7E3372-0524-49B7-AA32-F12BEB3864D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="735" windowWidth="23985" windowHeight="14265" xr2:uid="{1421E284-CBF3-4912-9765-3F7D17EF0783}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{1421E284-CBF3-4912-9765-3F7D17EF0783}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -237,6 +237,31 @@
       </text>
     </comment>
     <comment ref="I1" authorId="0" shapeId="0" xr:uid="{9D9603A5-6ED9-4461-9057-2C7332180EE0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+-Mandatory
+-Please use the existing nomenclature as shown by CapHive</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{24AA15DC-4F9B-4FD8-BEEE-83BF68133357}">
       <text>
         <r>
           <rPr>
@@ -446,14 +471,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -775,7 +799,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4:J20"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -789,6 +813,7 @@
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.86328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.06640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.73046875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -819,7 +844,7 @@
       <c r="I1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1398,9 +1423,12 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576" xr:uid="{E4F543E0-B5B2-429B-9B62-7D17366B8716}">
       <formula1>"Pool,All"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576" xr:uid="{1DC8B0BC-311B-4A76-A00C-6EF935294A5D}">
+      <formula1>"Accounting,Reporting"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added account entries import with folio and fund currency
</commit_message>
<xml_diff>
--- a/public/sample_uploads/account_entries.xlsx
+++ b/public/sample_uploads/account_entries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aseem Karmali\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A7E3372-0524-49B7-AA32-F12BEB3864D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EFA2FD9-AF75-48D4-89E4-EA746A2B0878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{1421E284-CBF3-4912-9765-3F7D17EF0783}"/>
+    <workbookView xWindow="15" yWindow="735" windowWidth="23985" windowHeight="14265" xr2:uid="{1421E284-CBF3-4912-9765-3F7D17EF0783}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -212,7 +212,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{914B8BE3-84D1-4DA5-9E4C-1617DB28A883}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{914B8BE3-84D1-4DA5-9E4C-1617DB28A883}">
       <text>
         <r>
           <rPr>
@@ -236,7 +236,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{9D9603A5-6ED9-4461-9057-2C7332180EE0}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{9D9603A5-6ED9-4461-9057-2C7332180EE0}">
       <text>
         <r>
           <rPr>
@@ -261,7 +261,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{24AA15DC-4F9B-4FD8-BEEE-83BF68133357}">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{24AA15DC-4F9B-4FD8-BEEE-83BF68133357}">
       <text>
         <r>
           <rPr>
@@ -291,7 +291,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="29">
   <si>
     <t>Investor *</t>
   </si>
@@ -311,9 +311,6 @@
     <t>Name *</t>
   </si>
   <si>
-    <t>Amount *</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -375,6 +372,12 @@
   </si>
   <si>
     <t>Reporting</t>
+  </si>
+  <si>
+    <t>Amount (Fund Currency)*</t>
+  </si>
+  <si>
+    <t>Amount (Folio Currency)</t>
   </si>
 </sst>
 </file>
@@ -796,10 +799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFD405DB-DFFA-46CC-B3D6-72FB3274A2C6}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -810,13 +813,14 @@
     <col min="4" max="4" width="15.265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.53125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.19921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.86328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.06640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.73046875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.53125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.73046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.06640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.73046875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -836,24 +840,27 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+        <v>17</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2">
         <v>10</v>
@@ -862,28 +869,29 @@
         <v>45018</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G2" s="2">
         <v>0.06</v>
       </c>
       <c r="H2" s="2"/>
-      <c r="I2" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+        <v>18</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3">
         <v>6</v>
@@ -892,28 +900,29 @@
         <v>44987</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="G3" s="2">
         <v>1000</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="I3" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="I3" s="2"/>
       <c r="J3" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+        <v>18</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="3">
         <v>7</v>
@@ -922,30 +931,31 @@
         <v>44987</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="G4" s="2">
         <v>2000</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="H4" s="2"/>
       <c r="I4" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+        <v>18</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3">
         <v>7</v>
@@ -954,28 +964,29 @@
         <v>44987</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="G5" s="2">
         <v>1000</v>
       </c>
       <c r="H5" s="2"/>
-      <c r="I5" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="I5" s="2"/>
       <c r="J5" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+        <v>18</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="3">
         <v>8</v>
@@ -984,28 +995,29 @@
         <v>45018</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="G6" s="2">
         <v>1000</v>
       </c>
       <c r="H6" s="2"/>
-      <c r="I6" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="I6" s="2"/>
       <c r="J6" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+        <v>18</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="3">
         <v>9</v>
@@ -1014,30 +1026,31 @@
         <v>45018</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="G7" s="2">
         <v>2000</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="H7" s="2"/>
       <c r="I7" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+        <v>18</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="3">
         <v>9</v>
@@ -1046,28 +1059,29 @@
         <v>45018</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="G8" s="2">
         <v>1000</v>
       </c>
       <c r="H8" s="2"/>
-      <c r="I8" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="I8" s="2"/>
       <c r="J8" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+        <v>18</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="3">
         <v>10</v>
@@ -1076,28 +1090,29 @@
         <v>45018</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="G9" s="2">
         <v>1000</v>
       </c>
       <c r="H9" s="2"/>
-      <c r="I9" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="I9" s="2"/>
       <c r="J9" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+        <v>18</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="3">
         <v>6</v>
@@ -1106,28 +1121,29 @@
         <v>44987</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="G10" s="2">
         <v>500</v>
       </c>
       <c r="H10" s="2"/>
-      <c r="I10" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="I10" s="2"/>
       <c r="J10" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+        <v>18</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="3">
         <v>7</v>
@@ -1136,28 +1152,29 @@
         <v>44987</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="G11" s="2">
         <v>500</v>
       </c>
       <c r="H11" s="2"/>
-      <c r="I11" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="I11" s="2"/>
       <c r="J11" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+        <v>18</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="3">
         <v>8</v>
@@ -1166,28 +1183,29 @@
         <v>45018</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="G12" s="2">
         <v>500</v>
       </c>
       <c r="H12" s="2"/>
-      <c r="I12" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="I12" s="2"/>
       <c r="J12" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+        <v>18</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="3">
         <v>9</v>
@@ -1196,28 +1214,29 @@
         <v>45018</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="G13" s="2">
         <v>500</v>
       </c>
       <c r="H13" s="2"/>
-      <c r="I13" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="I13" s="2"/>
       <c r="J13" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+        <v>18</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="3">
         <v>10</v>
@@ -1226,28 +1245,29 @@
         <v>45018</v>
       </c>
       <c r="E14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="G14" s="2">
         <v>500</v>
       </c>
       <c r="H14" s="2"/>
-      <c r="I14" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="I14" s="2"/>
       <c r="J14" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+        <v>18</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" s="3">
         <v>6</v>
@@ -1256,28 +1276,29 @@
         <v>44987</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G15" s="2">
         <v>0.05</v>
       </c>
       <c r="H15" s="2"/>
-      <c r="I15" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="I15" s="2"/>
       <c r="J15" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+        <v>18</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="3">
         <v>7</v>
@@ -1286,28 +1307,29 @@
         <v>44987</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G16" s="2">
         <v>0.06</v>
       </c>
       <c r="H16" s="2"/>
-      <c r="I16" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="I16" s="2"/>
       <c r="J16" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+        <v>18</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" s="3">
         <v>8</v>
@@ -1316,28 +1338,29 @@
         <v>45018</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G17" s="2">
         <v>0.05</v>
       </c>
       <c r="H17" s="2"/>
-      <c r="I17" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="I17" s="2"/>
       <c r="J17" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+        <v>18</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="3">
         <v>9</v>
@@ -1346,28 +1369,29 @@
         <v>45018</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G18" s="2">
         <v>0.06</v>
       </c>
       <c r="H18" s="2"/>
-      <c r="I18" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="I18" s="2"/>
       <c r="J18" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+        <v>18</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" s="3">
         <v>11</v>
@@ -1376,28 +1400,29 @@
         <v>45018</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G19" s="2">
         <v>0.06</v>
       </c>
       <c r="H19" s="2"/>
-      <c r="I19" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="I19" s="2"/>
       <c r="J19" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+        <v>18</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C20" s="3">
         <v>12</v>
@@ -1406,28 +1431,29 @@
         <v>45018</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G20" s="2">
         <v>0.06</v>
       </c>
       <c r="H20" s="2"/>
-      <c r="I20" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="I20" s="2"/>
       <c r="J20" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576" xr:uid="{E4F543E0-B5B2-429B-9B62-7D17366B8716}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576" xr:uid="{E4F543E0-B5B2-429B-9B62-7D17366B8716}">
       <formula1>"Pool,All"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576" xr:uid="{1DC8B0BC-311B-4A76-A00C-6EF935294A5D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576" xr:uid="{1DC8B0BC-311B-4A76-A00C-6EF935294A5D}">
       <formula1>"Accounting,Reporting"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update sample excel files (#715)
* Added updated xls for remittance, remit payments, commitments and AEs

* Fixed referrer nil issue in ransack header
</commit_message>
<xml_diff>
--- a/public/sample_uploads/account_entries.xlsx
+++ b/public/sample_uploads/account_entries.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f10f76f200b1328/Desktop/Test/bulk files with notes/feb 25/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EFA2FD9-AF75-48D4-89E4-EA746A2B0878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{7EFA2FD9-AF75-48D4-89E4-EA746A2B0878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8131789D-5A2B-4A1E-AE67-D07A0DA591FD}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="735" windowWidth="23985" windowHeight="14265" xr2:uid="{1421E284-CBF3-4912-9765-3F7D17EF0783}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{1421E284-CBF3-4912-9765-3F7D17EF0783}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -209,6 +209,30 @@
           <t xml:space="preserve">
 -Mandatory
 -Incase of a percentage - please put the exact value i.e. 0.06 for 6%</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{AAB58F6B-A23E-4AE8-8BFD-BC12393DDD01}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Leave blank if you want the system to convert based on FX rates entered by you in the system</t>
         </r>
       </text>
     </comment>
@@ -802,7 +826,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -814,7 +838,7 @@
     <col min="5" max="5" width="11.53125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.19921875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.53125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.73046875" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="8.86328125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.06640625" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.73046875" style="2" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Removed Type from imports
</commit_message>
<xml_diff>
--- a/public/sample_uploads/account_entries.xlsx
+++ b/public/sample_uploads/account_entries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f10f76f200b1328/Desktop/Test/bulk files with notes/feb 25/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{7EFA2FD9-AF75-48D4-89E4-EA746A2B0878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8131789D-5A2B-4A1E-AE67-D07A0DA591FD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB67AD2-7248-49E2-8CC5-748930339B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{1421E284-CBF3-4912-9765-3F7D17EF0783}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{1421E284-CBF3-4912-9765-3F7D17EF0783}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -260,32 +260,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{9D9603A5-6ED9-4461-9057-2C7332180EE0}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
--Mandatory
--Please use the existing nomenclature as shown by CapHive</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{24AA15DC-4F9B-4FD8-BEEE-83BF68133357}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{24AA15DC-4F9B-4FD8-BEEE-83BF68133357}">
       <text>
         <r>
           <rPr>
@@ -315,7 +290,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="27">
   <si>
     <t>Investor *</t>
   </si>
@@ -366,12 +341,6 @@
   </si>
   <si>
     <t>Investor 4</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Pool</t>
   </si>
   <si>
     <t>Fees</t>
@@ -823,10 +792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFD405DB-DFFA-46CC-B3D6-72FB3274A2C6}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -840,11 +809,10 @@
     <col min="7" max="7" width="23.53125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.73046875" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="8.86328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.06640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.73046875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.73046875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -864,22 +832,19 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -893,10 +858,10 @@
         <v>45018</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="G2" s="2">
         <v>0.06</v>
@@ -904,13 +869,10 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -935,13 +897,10 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
@@ -968,13 +927,10 @@
         <v>11</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -999,13 +955,10 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
@@ -1030,13 +983,10 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
@@ -1063,13 +1013,10 @@
         <v>11</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -1094,13 +1041,10 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -1125,13 +1069,10 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -1145,10 +1086,10 @@
         <v>44987</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G10" s="2">
         <v>500</v>
@@ -1156,13 +1097,10 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
@@ -1176,10 +1114,10 @@
         <v>44987</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G11" s="2">
         <v>500</v>
@@ -1187,13 +1125,10 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>15</v>
       </c>
@@ -1207,10 +1142,10 @@
         <v>45018</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G12" s="2">
         <v>500</v>
@@ -1218,13 +1153,10 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
@@ -1238,10 +1170,10 @@
         <v>45018</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G13" s="2">
         <v>500</v>
@@ -1249,13 +1181,10 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>16</v>
       </c>
@@ -1269,10 +1198,10 @@
         <v>45018</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G14" s="2">
         <v>500</v>
@@ -1280,13 +1209,10 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>12</v>
       </c>
@@ -1300,10 +1226,10 @@
         <v>44987</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="G15" s="2">
         <v>0.05</v>
@@ -1311,13 +1237,10 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
@@ -1331,10 +1254,10 @@
         <v>44987</v>
       </c>
       <c r="E16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="G16" s="2">
         <v>0.06</v>
@@ -1342,13 +1265,10 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -1362,10 +1282,10 @@
         <v>45018</v>
       </c>
       <c r="E17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="G17" s="2">
         <v>0.05</v>
@@ -1373,13 +1293,10 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
@@ -1393,10 +1310,10 @@
         <v>45018</v>
       </c>
       <c r="E18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="G18" s="2">
         <v>0.06</v>
@@ -1404,15 +1321,12 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>13</v>
@@ -1424,10 +1338,10 @@
         <v>45018</v>
       </c>
       <c r="E19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="G19" s="2">
         <v>0.06</v>
@@ -1435,15 +1349,12 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>13</v>
@@ -1455,10 +1366,10 @@
         <v>45018</v>
       </c>
       <c r="E20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="G20" s="2">
         <v>0.06</v>
@@ -1466,18 +1377,12 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576" xr:uid="{E4F543E0-B5B2-429B-9B62-7D17366B8716}">
-      <formula1>"Pool,All"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576" xr:uid="{1DC8B0BC-311B-4A76-A00C-6EF935294A5D}">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576" xr:uid="{1DC8B0BC-311B-4A76-A00C-6EF935294A5D}">
       <formula1>"Accounting,Reporting"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>